<commit_message>
Mise à jour des données
</commit_message>
<xml_diff>
--- a/src/docs/snt/04-donnees-structurees/assets/liste_des_films_plus_million_entrees.xlsx
+++ b/src/docs/snt/04-donnees-structurees/assets/liste_des_films_plus_million_entrees.xlsx
@@ -1,53 +1,54 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\groupe\BO\ETUDOC\SITE INTERNET CNC\Cinéma\Fréquentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CD2207B-13A9-457E-8C7C-0BF1049EF270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F5D001-05B5-44D6-8FC2-1DB3947E3016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="11" r:id="rId1"/>
-    <sheet name="2022" sheetId="24" r:id="rId2"/>
-    <sheet name="2021" sheetId="23" r:id="rId3"/>
-    <sheet name="2020" sheetId="22" r:id="rId4"/>
-    <sheet name="2019" sheetId="21" r:id="rId5"/>
-    <sheet name="2018" sheetId="20" r:id="rId6"/>
-    <sheet name="2017" sheetId="18" r:id="rId7"/>
-    <sheet name="2016" sheetId="17" r:id="rId8"/>
-    <sheet name="2015" sheetId="16" r:id="rId9"/>
-    <sheet name="2014" sheetId="14" r:id="rId10"/>
-    <sheet name="2013" sheetId="13" r:id="rId11"/>
-    <sheet name="2012" sheetId="2" r:id="rId12"/>
-    <sheet name="2011" sheetId="3" r:id="rId13"/>
-    <sheet name="2010" sheetId="1" r:id="rId14"/>
-    <sheet name="2009" sheetId="4" r:id="rId15"/>
-    <sheet name="2008" sheetId="5" r:id="rId16"/>
-    <sheet name="2007" sheetId="6" r:id="rId17"/>
-    <sheet name="2006" sheetId="7" r:id="rId18"/>
-    <sheet name="2005" sheetId="8" r:id="rId19"/>
-    <sheet name="2004" sheetId="9" r:id="rId20"/>
-    <sheet name="2003" sheetId="10" r:id="rId21"/>
-    <sheet name="ESRI_MAPINFO_SHEET" sheetId="19" state="veryHidden" r:id="rId22"/>
+    <sheet name="2023" sheetId="25" r:id="rId2"/>
+    <sheet name="2022" sheetId="24" r:id="rId3"/>
+    <sheet name="2021" sheetId="23" r:id="rId4"/>
+    <sheet name="2020" sheetId="22" r:id="rId5"/>
+    <sheet name="2019" sheetId="21" r:id="rId6"/>
+    <sheet name="2018" sheetId="20" r:id="rId7"/>
+    <sheet name="2017" sheetId="18" r:id="rId8"/>
+    <sheet name="2016" sheetId="17" r:id="rId9"/>
+    <sheet name="2015" sheetId="16" r:id="rId10"/>
+    <sheet name="2014" sheetId="14" r:id="rId11"/>
+    <sheet name="2013" sheetId="13" r:id="rId12"/>
+    <sheet name="2012" sheetId="2" r:id="rId13"/>
+    <sheet name="2011" sheetId="3" r:id="rId14"/>
+    <sheet name="2010" sheetId="1" r:id="rId15"/>
+    <sheet name="2009" sheetId="4" r:id="rId16"/>
+    <sheet name="2008" sheetId="5" r:id="rId17"/>
+    <sheet name="2007" sheetId="6" r:id="rId18"/>
+    <sheet name="2006" sheetId="7" r:id="rId19"/>
+    <sheet name="2005" sheetId="8" r:id="rId20"/>
+    <sheet name="2004" sheetId="9" r:id="rId21"/>
+    <sheet name="2003" sheetId="10" r:id="rId22"/>
+    <sheet name="ESRI_MAPINFO_SHEET" sheetId="19" state="veryHidden" r:id="rId23"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'2012'!$A$7:$E$60</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'2013'!$A$7:$E$62</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'2014'!$A$7:$E$64</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'2015'!$A$7:$E$52</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'2016'!$A$7:$E$61</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'2017'!$A$7:$E$63</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'2018'!$A$7:$E$49</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'2019'!$A$7:$E$58</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2021'!$A$7:$E$32</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="13">'2010'!$5:$7</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="13">'2010'!$A$5:$E$59</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'2012'!$A$7:$E$60</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'2013'!$A$7:$E$62</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'2014'!$A$7:$E$64</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'2015'!$A$7:$E$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'2016'!$A$7:$E$61</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'2017'!$A$7:$E$63</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'2018'!$A$7:$E$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'2019'!$A$7:$E$58</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2021'!$A$7:$E$32</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="14">'2010'!$5:$7</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="14">'2010'!$A$5:$E$59</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1918" uniqueCount="951">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2014" uniqueCount="995">
   <si>
     <t>titre</t>
   </si>
@@ -2760,24 +2761,12 @@
     <t>DUNE</t>
   </si>
   <si>
-    <t>KAAMELOTT VOLET 1</t>
-  </si>
-  <si>
     <t>BAC NORD</t>
   </si>
   <si>
     <t>ENCANTO, LA FANTASTIQUE FAMILLE MADRIGAL</t>
   </si>
   <si>
-    <t>FAST &amp; FURIOUS 9</t>
-  </si>
-  <si>
-    <t>TUCHE 4 (LES)</t>
-  </si>
-  <si>
-    <t>CONJURING 3: THE DEVIL MADE ME DO IT</t>
-  </si>
-  <si>
     <t>LES ETERNELS</t>
   </si>
   <si>
@@ -2790,18 +2779,12 @@
     <t>OSS 117 - ALERTE ROUGE EN AFRIQUE NOIRE</t>
   </si>
   <si>
-    <t>BODIN'S AU PAYS DU SOURIRE (LES)</t>
-  </si>
-  <si>
     <t>EIFFEL</t>
   </si>
   <si>
     <t>FR/DE</t>
   </si>
   <si>
-    <t>PAT'PATROUILLE - LE FILM (LA)</t>
-  </si>
-  <si>
     <t>CRUELLA</t>
   </si>
   <si>
@@ -2820,9 +2803,6 @@
     <t>BOITE NOIRE</t>
   </si>
   <si>
-    <t>LOUP ET LE LION (LE)</t>
-  </si>
-  <si>
     <t>TOUS EN SCENE 2</t>
   </si>
   <si>
@@ -2916,18 +2896,175 @@
     <t>LES BAD GUYS</t>
   </si>
   <si>
-    <t>Mis à jour le 19 juin 2023</t>
+    <t>Mis à jour le 22 mai 2024</t>
+  </si>
+  <si>
+    <t>SUPER MARIO BROS. LE FILM</t>
+  </si>
+  <si>
+    <t>BARBIE</t>
+  </si>
+  <si>
+    <t>ASTERIX ET OBELIX ET L'EMPIRE DU MILIEU</t>
+  </si>
+  <si>
+    <t>OPPENHEIMER</t>
+  </si>
+  <si>
+    <t>ALIBI.COM 2</t>
+  </si>
+  <si>
+    <t>LES GARDIENS DE LA GALAXIE : VOLUME 3</t>
+  </si>
+  <si>
+    <t>LES TROIS MOUSQUETAIRES - D'ARTAGNAN</t>
+  </si>
+  <si>
+    <t>ELEMENTAIRE</t>
+  </si>
+  <si>
+    <t>INDIANA JONES ET LE CADRAN DE LA DESTINEE</t>
+  </si>
+  <si>
+    <t>MISSION IMPOSSIBLE DEAD RECKONING PARTIE 1</t>
+  </si>
+  <si>
+    <t>PAW PATROL : LA SUPER PATROUILLE - LE FILM</t>
+  </si>
+  <si>
+    <t>CREED III</t>
+  </si>
+  <si>
+    <t>FAST &amp; FURIOUS X</t>
+  </si>
+  <si>
+    <t>WONKA</t>
+  </si>
+  <si>
+    <t>WISH, ASHA ET LA BONNE ETOILE</t>
+  </si>
+  <si>
+    <t>SPIDER-MAN : ACROSS THE SPIDER-VERSE</t>
+  </si>
+  <si>
+    <t>3 JOURS MAX</t>
+  </si>
+  <si>
+    <t>LA PETITE SIRENE</t>
+  </si>
+  <si>
+    <t>LES TROIS MOUSQUETAIRES - MILADY</t>
+  </si>
+  <si>
+    <t>EN EAUX TRES TROUBLES</t>
+  </si>
+  <si>
+    <t>CN</t>
+  </si>
+  <si>
+    <t>MIRACULOUS LE FILM</t>
+  </si>
+  <si>
+    <t>HUNGER GAMES : LA BALLADE DU SERPENT ET DE L'OISEAU CHANTEUR</t>
+  </si>
+  <si>
+    <t>NAPOLEON</t>
+  </si>
+  <si>
+    <t>ANT-MAN ET LA GUEPE : QUANTUMANIA</t>
+  </si>
+  <si>
+    <t>LE GARCON ET LE HERON</t>
+  </si>
+  <si>
+    <t>JP</t>
+  </si>
+  <si>
+    <t>BABYLON</t>
+  </si>
+  <si>
+    <t>LES TROLLS 3</t>
+  </si>
+  <si>
+    <t>ANATOMIE D'UNE CHUTE</t>
+  </si>
+  <si>
+    <t>KILLERS OF THE FLOWER MOON</t>
+  </si>
+  <si>
+    <t>TIRAILLEURS</t>
+  </si>
+  <si>
+    <t>FR / SN</t>
+  </si>
+  <si>
+    <t>SCREAM VI</t>
+  </si>
+  <si>
+    <t>DONJONS &amp; DRAGONS : L'HONNEUR DES VOLEURS</t>
+  </si>
+  <si>
+    <t>JE VERRAI TOUJOURS VOS VISAGES</t>
+  </si>
+  <si>
+    <t>GRAN TURISMO</t>
+  </si>
+  <si>
+    <t>LA NONNE 2</t>
+  </si>
+  <si>
+    <t>TRANSFORMERS : RISE OF THE BEASTS</t>
+  </si>
+  <si>
+    <t>AQUAMAN ET LE ROYAUME PERDU</t>
+  </si>
+  <si>
+    <t>MON CRIME</t>
+  </si>
+  <si>
+    <t>LE REGNE ANIMAL</t>
+  </si>
+  <si>
+    <t>SUR LES CHEMINS NOIRS</t>
+  </si>
+  <si>
+    <t>JOHN WICK : CHAPITRE 4</t>
+  </si>
+  <si>
+    <t>KAAMELOTT - PREMIER VOLET</t>
+  </si>
+  <si>
+    <t>FAST AND FURIOUS 9</t>
+  </si>
+  <si>
+    <t>LES TUCHE 4</t>
+  </si>
+  <si>
+    <t>CONJURING 3 SOUS L'EMPRISE DU DIABLE</t>
+  </si>
+  <si>
+    <t>LES BODIN'S EN THAILANDE</t>
+  </si>
+  <si>
+    <t>PAW PATROL - LE FILM - LA PAT PATROUILLE</t>
+  </si>
+  <si>
+    <t>LE LOUP ET LE LION</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="#,##0.00,,"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="169" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="9"/>
       <name val="Arial"/>
@@ -3041,6 +3178,16 @@
       <color theme="8"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -3377,9 +3524,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3417,9 +3564,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3452,26 +3599,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3504,26 +3634,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3697,10 +3810,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A5:B28"/>
+  <dimension ref="A5:B29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -3715,7 +3828,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="43" t="s">
-        <v>950</v>
+        <v>943</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -3724,126 +3837,133 @@
     <row r="9" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="43"/>
       <c r="B9" s="36">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="43"/>
+      <c r="B10" s="36">
         <v>2022</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" s="36" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="36">
-        <v>2021</v>
       </c>
     </row>
     <row r="11" spans="1:2" s="36" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="36">
-        <v>2020</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="12" spans="1:2" s="36" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="36">
-        <v>2019</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="13" spans="1:2" s="36" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="36">
-        <v>2018</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="14" spans="1:2" s="36" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="36">
-        <v>2017</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="15" spans="1:2" s="36" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="36">
-        <v>2016</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="16" spans="1:2" s="36" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="36">
-        <v>2015</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="17" spans="2:2" s="36" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="36">
-        <v>2014</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="18" spans="2:2" s="36" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="36">
-        <v>2013</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="19" spans="2:2" s="36" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="36">
-        <v>2012</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="20" spans="2:2" s="36" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="36">
-        <v>2011</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="21" spans="2:2" s="36" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="36">
-        <v>2010</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="22" spans="2:2" s="36" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="36">
-        <v>2009</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="23" spans="2:2" s="36" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="36">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="24" spans="2:2" s="36" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="36">
-        <v>2007</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="25" spans="2:2" s="36" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="36">
-        <v>2006</v>
+        <v>2007</v>
       </c>
     </row>
     <row r="26" spans="2:2" s="36" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="36">
-        <v>2005</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="27" spans="2:2" s="36" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="36">
-        <v>2004</v>
+        <v>2005</v>
       </c>
     </row>
     <row r="28" spans="2:2" s="36" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="36">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" s="36" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="36">
         <v>2003</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B19" location="'2012'!A1" display="'2012'!A1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B20" location="'2011'!A1" display="'2011'!A1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B21" location="'2010'!A1" display="'2010'!A1" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B23" location="'2008'!A1" display="'2008'!A1" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B25" location="'2006'!A1" display="'2006'!A1" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B27" location="'2004'!A1" display="'2004'!A1" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B22" location="'2009'!A1" display="'2009'!A1" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B24" location="'2007'!A1" display="'2007'!A1" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B26" location="'2005'!A1" display="'2005'!A1" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B28" location="'2003'!A1" display="'2003'!A1" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B18" location="'2013'!A1" display="'2013'!A1" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B17" location="'2014'!A1" display="'2014'!A1" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B16" location="'2015'!A1" display="'2015'!A1" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B15" location="'2016'!A1" display="'2016'!A1" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B14" location="'2017'!A1" display="'2017'!A1" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B13" location="'2018'!A1" display="'2018'!A1" xr:uid="{6EE7A24B-096B-43FF-BFDB-0286DA2B4B53}"/>
-    <hyperlink ref="B12" location="'2019'!A1" display="'2019'!A1" xr:uid="{ED3570CA-B57F-4DE6-8B10-03F4FFCCFC95}"/>
-    <hyperlink ref="B11" location="'2020'!A1" display="'2020'!A1" xr:uid="{00FF75B9-CAC3-47AB-B072-9DE1FB91ED7E}"/>
-    <hyperlink ref="B10" location="'2021'!A1" display="'2021'!A1" xr:uid="{73AEEB73-E0B9-4AB4-9DE9-3A0CAE484A5A}"/>
-    <hyperlink ref="B9" location="'2022'!A1" display="'2022'!A1" xr:uid="{B96B8336-0E48-4587-8E74-5A9F687C802F}"/>
+    <hyperlink ref="B20" location="'2012'!A1" display="'2012'!A1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B21" location="'2011'!A1" display="'2011'!A1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B22" location="'2010'!A1" display="'2010'!A1" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B24" location="'2008'!A1" display="'2008'!A1" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B26" location="'2006'!A1" display="'2006'!A1" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B28" location="'2004'!A1" display="'2004'!A1" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B23" location="'2009'!A1" display="'2009'!A1" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B25" location="'2007'!A1" display="'2007'!A1" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B27" location="'2005'!A1" display="'2005'!A1" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B29" location="'2003'!A1" display="'2003'!A1" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B19" location="'2013'!A1" display="'2013'!A1" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B18" location="'2014'!A1" display="'2014'!A1" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B17" location="'2015'!A1" display="'2015'!A1" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B16" location="'2016'!A1" display="'2016'!A1" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B15" location="'2017'!A1" display="'2017'!A1" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B14" location="'2018'!A1" display="'2018'!A1" xr:uid="{6EE7A24B-096B-43FF-BFDB-0286DA2B4B53}"/>
+    <hyperlink ref="B13" location="'2019'!A1" display="'2019'!A1" xr:uid="{ED3570CA-B57F-4DE6-8B10-03F4FFCCFC95}"/>
+    <hyperlink ref="B12" location="'2020'!A1" display="'2020'!A1" xr:uid="{00FF75B9-CAC3-47AB-B072-9DE1FB91ED7E}"/>
+    <hyperlink ref="B11" location="'2021'!A1" display="'2021'!A1" xr:uid="{73AEEB73-E0B9-4AB4-9DE9-3A0CAE484A5A}"/>
+    <hyperlink ref="B10" location="'2022'!A1" display="'2022'!A1" xr:uid="{B96B8336-0E48-4587-8E74-5A9F687C802F}"/>
+    <hyperlink ref="B9" location="'2023'!A1" display="'2023'!A1" xr:uid="{3EB4CFD3-29A7-4017-B703-C0C3FBE28CA0}"/>
   </hyperlinks>
   <pageMargins left="0.59055118110236227" right="0.59055118110236227" top="0.78740157480314965" bottom="0.78740157480314965" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" scale="90" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -3853,6 +3973,846 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:E52"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.28515625" style="24" customWidth="1"/>
+    <col min="2" max="2" width="50.28515625" style="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" style="34" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" style="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" style="27" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" s="37" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="41"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+    </row>
+    <row r="3" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="6">
+        <v>2015</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="9"/>
+    </row>
+    <row r="6" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="6"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="9"/>
+    </row>
+    <row r="7" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>633</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="16">
+        <v>1</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>634</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="18">
+        <v>42354</v>
+      </c>
+      <c r="E8" s="19">
+        <v>7327435</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="16">
+        <v>2</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>716</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="18">
+        <v>42193</v>
+      </c>
+      <c r="E9" s="19">
+        <v>6655855</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="16">
+        <v>3</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>717</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="18">
+        <v>41990</v>
+      </c>
+      <c r="E10" s="19">
+        <v>5351811</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="16">
+        <v>4</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>635</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="18">
+        <v>42165</v>
+      </c>
+      <c r="E11" s="19">
+        <v>5214046</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="16">
+        <v>5</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>636</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="18">
+        <v>42319</v>
+      </c>
+      <c r="E12" s="19">
+        <v>4813082</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="16">
+        <v>6</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>637</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="18">
+        <v>42095</v>
+      </c>
+      <c r="E13" s="19">
+        <v>4631125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="16">
+        <v>7</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>718</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="18">
+        <v>42291</v>
+      </c>
+      <c r="E14" s="19">
+        <v>4426102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="16">
+        <v>8</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>638</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="18">
+        <v>42172</v>
+      </c>
+      <c r="E15" s="19">
+        <v>4410201</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="16">
+        <v>9</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>639</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="18">
+        <v>42116</v>
+      </c>
+      <c r="E16" s="19">
+        <v>4240121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="16">
+        <v>10</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>640</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="18">
+        <v>42046</v>
+      </c>
+      <c r="E17" s="19">
+        <v>4065415</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="16">
+        <v>11</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>719</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="18">
+        <v>42186</v>
+      </c>
+      <c r="E18" s="19">
+        <v>3494441</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="16">
+        <v>12</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>641</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="18">
+        <v>42053</v>
+      </c>
+      <c r="E19" s="19">
+        <v>3132953</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="16">
+        <v>13</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>720</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="18">
+        <v>42284</v>
+      </c>
+      <c r="E20" s="19">
+        <v>3122000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="16">
+        <v>14</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>642</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="18">
+        <v>42039</v>
+      </c>
+      <c r="E21" s="19">
+        <v>2887691</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="16">
+        <v>15</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>643</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="18">
+        <v>42228</v>
+      </c>
+      <c r="E22" s="19">
+        <v>2797975</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="16">
+        <v>16</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>721</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="18">
+        <v>42326</v>
+      </c>
+      <c r="E23" s="19">
+        <v>2773963</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="16">
+        <v>17</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>644</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="18">
+        <v>42025</v>
+      </c>
+      <c r="E24" s="19">
+        <v>2612213</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="16">
+        <v>18</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>645</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="18">
+        <v>42340</v>
+      </c>
+      <c r="E25" s="19">
+        <v>2525612</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="16">
+        <v>19</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>646</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="18">
+        <v>42298</v>
+      </c>
+      <c r="E26" s="19">
+        <v>2519790</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="16">
+        <v>20</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>647</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="18">
+        <v>42081</v>
+      </c>
+      <c r="E27" s="19">
+        <v>2417013</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="16">
+        <v>21</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>648</v>
+      </c>
+      <c r="C28" s="29" t="s">
+        <v>170</v>
+      </c>
+      <c r="D28" s="18">
+        <v>42102</v>
+      </c>
+      <c r="E28" s="19">
+        <v>2410643</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="16">
+        <v>22</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>649</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="D29" s="18">
+        <v>42138</v>
+      </c>
+      <c r="E29" s="19">
+        <v>2359477</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="16">
+        <v>23</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>722</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="18">
+        <v>42333</v>
+      </c>
+      <c r="E30" s="19">
+        <v>2316475</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="16">
+        <v>24</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>650</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="18">
+        <v>42284</v>
+      </c>
+      <c r="E31" s="19">
+        <v>2298078</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="16">
+        <v>25</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>723</v>
+      </c>
+      <c r="C32" s="29" t="s">
+        <v>170</v>
+      </c>
+      <c r="D32" s="18">
+        <v>42214</v>
+      </c>
+      <c r="E32" s="19">
+        <v>1934437</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="16">
+        <v>26</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>651</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="18">
+        <v>42199</v>
+      </c>
+      <c r="E33" s="19">
+        <v>1721905</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="16">
+        <v>27</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>652</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="18">
+        <v>42088</v>
+      </c>
+      <c r="E34" s="19">
+        <v>1674276</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="16">
+        <v>28</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>653</v>
+      </c>
+      <c r="C35" s="29" t="s">
+        <v>729</v>
+      </c>
+      <c r="D35" s="18">
+        <v>42053</v>
+      </c>
+      <c r="E35" s="19">
+        <v>1666999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="16">
+        <v>29</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>724</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" s="18">
+        <v>42046</v>
+      </c>
+      <c r="E36" s="19">
+        <v>1660709</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="16">
+        <v>30</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>725</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" s="18">
+        <v>42039</v>
+      </c>
+      <c r="E37" s="19">
+        <v>1591922</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="16">
+        <v>31</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>654</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" s="18">
+        <v>42053</v>
+      </c>
+      <c r="E38" s="19">
+        <v>1512366</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="16">
+        <v>32</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>655</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="18">
+        <v>42186</v>
+      </c>
+      <c r="E39" s="19">
+        <v>1425869</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="16">
+        <v>33</v>
+      </c>
+      <c r="B40" s="17" t="s">
+        <v>726</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" s="18">
+        <v>42347</v>
+      </c>
+      <c r="E40" s="19">
+        <v>1369011</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="16">
+        <v>34</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>727</v>
+      </c>
+      <c r="C41" s="29" t="s">
+        <v>730</v>
+      </c>
+      <c r="D41" s="18">
+        <v>42060</v>
+      </c>
+      <c r="E41" s="19">
+        <v>1326539</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="16">
+        <v>35</v>
+      </c>
+      <c r="B42" s="17" t="s">
+        <v>656</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" s="18">
+        <v>42053</v>
+      </c>
+      <c r="E42" s="19">
+        <v>1300935</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="16">
+        <v>36</v>
+      </c>
+      <c r="B43" s="17" t="s">
+        <v>657</v>
+      </c>
+      <c r="C43" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" s="18">
+        <v>42109</v>
+      </c>
+      <c r="E43" s="19">
+        <v>1224306</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="16">
+        <v>37</v>
+      </c>
+      <c r="B44" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44" s="18">
+        <v>42221</v>
+      </c>
+      <c r="E44" s="19">
+        <v>1204400</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="16">
+        <v>38</v>
+      </c>
+      <c r="B45" s="17" t="s">
+        <v>658</v>
+      </c>
+      <c r="C45" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D45" s="18">
+        <v>42123</v>
+      </c>
+      <c r="E45" s="19">
+        <v>1199076</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="16">
+        <v>39</v>
+      </c>
+      <c r="B46" s="17" t="s">
+        <v>659</v>
+      </c>
+      <c r="C46" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46" s="18">
+        <v>42151</v>
+      </c>
+      <c r="E46" s="19">
+        <v>1151362</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="16">
+        <v>40</v>
+      </c>
+      <c r="B47" s="17" t="s">
+        <v>660</v>
+      </c>
+      <c r="C47" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D47" s="18">
+        <v>42221</v>
+      </c>
+      <c r="E47" s="19">
+        <v>1143896</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="16">
+        <v>41</v>
+      </c>
+      <c r="B48" s="17" t="s">
+        <v>661</v>
+      </c>
+      <c r="C48" s="29" t="s">
+        <v>729</v>
+      </c>
+      <c r="D48" s="18">
+        <v>42032</v>
+      </c>
+      <c r="E48" s="19">
+        <v>1088829</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="16">
+        <v>42</v>
+      </c>
+      <c r="B49" s="17" t="s">
+        <v>662</v>
+      </c>
+      <c r="C49" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49" s="18">
+        <v>42095</v>
+      </c>
+      <c r="E49" s="19">
+        <v>1063446</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="16">
+        <v>43</v>
+      </c>
+      <c r="B50" s="17" t="s">
+        <v>728</v>
+      </c>
+      <c r="C50" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="D50" s="18">
+        <v>42018</v>
+      </c>
+      <c r="E50" s="19">
+        <v>1062983</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="16">
+        <v>44</v>
+      </c>
+      <c r="B51" s="17" t="s">
+        <v>663</v>
+      </c>
+      <c r="C51" s="29" t="s">
+        <v>731</v>
+      </c>
+      <c r="D51" s="18">
+        <v>42263</v>
+      </c>
+      <c r="E51" s="19">
+        <v>1008223</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="23"/>
+      <c r="C52" s="34" t="s">
+        <v>732</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" location="Sommaire!A1" display="Retour au menu &quot;Films en salles&quot;" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E65"/>
   <sheetViews>
@@ -4908,7 +5868,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E63"/>
   <sheetViews>
@@ -5928,7 +6888,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E61"/>
   <sheetViews>
@@ -6914,7 +7874,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E61"/>
   <sheetViews>
@@ -7900,7 +8860,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E59"/>
   <sheetViews>
@@ -8858,7 +9818,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:E58"/>
   <sheetViews>
@@ -9793,7 +10753,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:E54"/>
   <sheetViews>
@@ -10660,7 +11620,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:E48"/>
   <sheetViews>
@@ -11425,7 +12385,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:E51"/>
   <sheetViews>
@@ -12241,7 +13201,788 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99A66032-C253-481F-AEDD-9BBB731EFA8E}">
+  <dimension ref="A2:E50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.28515625" customWidth="1"/>
+    <col min="2" max="2" width="50.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="37" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="45">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>633</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="46">
+        <v>1</v>
+      </c>
+      <c r="B8" s="47" t="s">
+        <v>944</v>
+      </c>
+      <c r="C8" s="47" t="s">
+        <v>784</v>
+      </c>
+      <c r="D8" s="48">
+        <v>45021</v>
+      </c>
+      <c r="E8" s="49">
+        <v>7249542</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="46">
+        <v>2</v>
+      </c>
+      <c r="B9" s="47" t="s">
+        <v>945</v>
+      </c>
+      <c r="C9" s="47" t="s">
+        <v>574</v>
+      </c>
+      <c r="D9" s="48">
+        <v>45126</v>
+      </c>
+      <c r="E9" s="49">
+        <v>5871888</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="46">
+        <v>3</v>
+      </c>
+      <c r="B10" s="47" t="s">
+        <v>916</v>
+      </c>
+      <c r="C10" s="47" t="s">
+        <v>784</v>
+      </c>
+      <c r="D10" s="48">
+        <v>44909</v>
+      </c>
+      <c r="E10" s="49">
+        <v>5219000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="46">
+        <v>4</v>
+      </c>
+      <c r="B11" s="47" t="s">
+        <v>946</v>
+      </c>
+      <c r="C11" s="47" t="s">
+        <v>785</v>
+      </c>
+      <c r="D11" s="48">
+        <v>44958</v>
+      </c>
+      <c r="E11" s="49">
+        <v>4605168</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="46">
+        <v>5</v>
+      </c>
+      <c r="B12" s="47" t="s">
+        <v>947</v>
+      </c>
+      <c r="C12" s="47" t="s">
+        <v>784</v>
+      </c>
+      <c r="D12" s="48">
+        <v>45126</v>
+      </c>
+      <c r="E12" s="49">
+        <v>4461566</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="46">
+        <v>6</v>
+      </c>
+      <c r="B13" s="47" t="s">
+        <v>948</v>
+      </c>
+      <c r="C13" s="47" t="s">
+        <v>785</v>
+      </c>
+      <c r="D13" s="48">
+        <v>44965</v>
+      </c>
+      <c r="E13" s="49">
+        <v>4282780</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="46">
+        <v>7</v>
+      </c>
+      <c r="B14" s="47" t="s">
+        <v>949</v>
+      </c>
+      <c r="C14" s="47" t="s">
+        <v>784</v>
+      </c>
+      <c r="D14" s="48">
+        <v>45049</v>
+      </c>
+      <c r="E14" s="49">
+        <v>3447513</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="46">
+        <v>8</v>
+      </c>
+      <c r="B15" s="47" t="s">
+        <v>950</v>
+      </c>
+      <c r="C15" s="47" t="s">
+        <v>785</v>
+      </c>
+      <c r="D15" s="48">
+        <v>45021</v>
+      </c>
+      <c r="E15" s="49">
+        <v>3435876</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="46">
+        <v>9</v>
+      </c>
+      <c r="B16" s="47" t="s">
+        <v>951</v>
+      </c>
+      <c r="C16" s="47" t="s">
+        <v>784</v>
+      </c>
+      <c r="D16" s="48">
+        <v>45098</v>
+      </c>
+      <c r="E16" s="49">
+        <v>3204072</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="46">
+        <v>10</v>
+      </c>
+      <c r="B17" s="47" t="s">
+        <v>952</v>
+      </c>
+      <c r="C17" s="47" t="s">
+        <v>784</v>
+      </c>
+      <c r="D17" s="48">
+        <v>45105</v>
+      </c>
+      <c r="E17" s="49">
+        <v>2955006</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="46">
+        <v>11</v>
+      </c>
+      <c r="B18" s="47" t="s">
+        <v>953</v>
+      </c>
+      <c r="C18" s="47" t="s">
+        <v>784</v>
+      </c>
+      <c r="D18" s="48">
+        <v>45119</v>
+      </c>
+      <c r="E18" s="49">
+        <v>2618065</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="46">
+        <v>12</v>
+      </c>
+      <c r="B19" s="47" t="s">
+        <v>954</v>
+      </c>
+      <c r="C19" s="47" t="s">
+        <v>784</v>
+      </c>
+      <c r="D19" s="48">
+        <v>45210</v>
+      </c>
+      <c r="E19" s="49">
+        <v>2312845</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="46">
+        <v>13</v>
+      </c>
+      <c r="B20" s="47" t="s">
+        <v>955</v>
+      </c>
+      <c r="C20" s="47" t="s">
+        <v>784</v>
+      </c>
+      <c r="D20" s="48">
+        <v>44986</v>
+      </c>
+      <c r="E20" s="49">
+        <v>2298291</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="46">
+        <v>14</v>
+      </c>
+      <c r="B21" s="47" t="s">
+        <v>956</v>
+      </c>
+      <c r="C21" s="47" t="s">
+        <v>574</v>
+      </c>
+      <c r="D21" s="48">
+        <v>45063</v>
+      </c>
+      <c r="E21" s="49">
+        <v>2270508</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="46">
+        <v>15</v>
+      </c>
+      <c r="B22" s="47" t="s">
+        <v>957</v>
+      </c>
+      <c r="C22" s="47" t="s">
+        <v>574</v>
+      </c>
+      <c r="D22" s="48">
+        <v>45273</v>
+      </c>
+      <c r="E22" s="49">
+        <v>2153203</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="46">
+        <v>16</v>
+      </c>
+      <c r="B23" s="47" t="s">
+        <v>958</v>
+      </c>
+      <c r="C23" s="47" t="s">
+        <v>784</v>
+      </c>
+      <c r="D23" s="48">
+        <v>45259</v>
+      </c>
+      <c r="E23" s="49">
+        <v>2131826</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="46">
+        <v>17</v>
+      </c>
+      <c r="B24" s="47" t="s">
+        <v>959</v>
+      </c>
+      <c r="C24" s="47" t="s">
+        <v>784</v>
+      </c>
+      <c r="D24" s="48">
+        <v>45077</v>
+      </c>
+      <c r="E24" s="49">
+        <v>1935229</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="46">
+        <v>18</v>
+      </c>
+      <c r="B25" s="47" t="s">
+        <v>960</v>
+      </c>
+      <c r="C25" s="47" t="s">
+        <v>785</v>
+      </c>
+      <c r="D25" s="48">
+        <v>45224</v>
+      </c>
+      <c r="E25" s="49">
+        <v>1886955</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="46">
+        <v>19</v>
+      </c>
+      <c r="B26" s="47" t="s">
+        <v>961</v>
+      </c>
+      <c r="C26" s="47" t="s">
+        <v>784</v>
+      </c>
+      <c r="D26" s="48">
+        <v>45070</v>
+      </c>
+      <c r="E26" s="49">
+        <v>1725558</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="46">
+        <v>20</v>
+      </c>
+      <c r="B27" s="47" t="s">
+        <v>962</v>
+      </c>
+      <c r="C27" s="47" t="s">
+        <v>785</v>
+      </c>
+      <c r="D27" s="48">
+        <v>45273</v>
+      </c>
+      <c r="E27" s="49">
+        <v>1681163</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="46">
+        <v>21</v>
+      </c>
+      <c r="B28" s="47" t="s">
+        <v>963</v>
+      </c>
+      <c r="C28" s="47" t="s">
+        <v>964</v>
+      </c>
+      <c r="D28" s="48">
+        <v>45140</v>
+      </c>
+      <c r="E28" s="49">
+        <v>1652599</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="46">
+        <v>22</v>
+      </c>
+      <c r="B29" s="47" t="s">
+        <v>965</v>
+      </c>
+      <c r="C29" s="47" t="s">
+        <v>785</v>
+      </c>
+      <c r="D29" s="48">
+        <v>45112</v>
+      </c>
+      <c r="E29" s="49">
+        <v>1645127</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="46">
+        <v>23</v>
+      </c>
+      <c r="B30" s="47" t="s">
+        <v>966</v>
+      </c>
+      <c r="C30" s="47" t="s">
+        <v>784</v>
+      </c>
+      <c r="D30" s="48">
+        <v>45245</v>
+      </c>
+      <c r="E30" s="49">
+        <v>1644265</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="46">
+        <v>24</v>
+      </c>
+      <c r="B31" s="47" t="s">
+        <v>967</v>
+      </c>
+      <c r="C31" s="47" t="s">
+        <v>784</v>
+      </c>
+      <c r="D31" s="48">
+        <v>45252</v>
+      </c>
+      <c r="E31" s="49">
+        <v>1603947</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="46">
+        <v>25</v>
+      </c>
+      <c r="B32" s="47" t="s">
+        <v>968</v>
+      </c>
+      <c r="C32" s="47" t="s">
+        <v>784</v>
+      </c>
+      <c r="D32" s="48">
+        <v>44972</v>
+      </c>
+      <c r="E32" s="49">
+        <v>1574000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="46">
+        <v>26</v>
+      </c>
+      <c r="B33" s="47" t="s">
+        <v>969</v>
+      </c>
+      <c r="C33" s="47" t="s">
+        <v>970</v>
+      </c>
+      <c r="D33" s="48">
+        <v>45231</v>
+      </c>
+      <c r="E33" s="49">
+        <v>1552271</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="46">
+        <v>27</v>
+      </c>
+      <c r="B34" s="47" t="s">
+        <v>971</v>
+      </c>
+      <c r="C34" s="47" t="s">
+        <v>784</v>
+      </c>
+      <c r="D34" s="48">
+        <v>44944</v>
+      </c>
+      <c r="E34" s="49">
+        <v>1511359</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="46">
+        <v>28</v>
+      </c>
+      <c r="B35" s="47" t="s">
+        <v>972</v>
+      </c>
+      <c r="C35" s="47" t="s">
+        <v>784</v>
+      </c>
+      <c r="D35" s="48">
+        <v>45217</v>
+      </c>
+      <c r="E35" s="49">
+        <v>1463921</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="46">
+        <v>29</v>
+      </c>
+      <c r="B36" s="47" t="s">
+        <v>973</v>
+      </c>
+      <c r="C36" s="47" t="s">
+        <v>785</v>
+      </c>
+      <c r="D36" s="48">
+        <v>45161</v>
+      </c>
+      <c r="E36" s="49">
+        <v>1299741</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="46">
+        <v>30</v>
+      </c>
+      <c r="B37" s="47" t="s">
+        <v>974</v>
+      </c>
+      <c r="C37" s="47" t="s">
+        <v>784</v>
+      </c>
+      <c r="D37" s="48">
+        <v>45217</v>
+      </c>
+      <c r="E37" s="49">
+        <v>1270406</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="46">
+        <v>31</v>
+      </c>
+      <c r="B38" s="47" t="s">
+        <v>975</v>
+      </c>
+      <c r="C38" s="47" t="s">
+        <v>976</v>
+      </c>
+      <c r="D38" s="48">
+        <v>44930</v>
+      </c>
+      <c r="E38" s="49">
+        <v>1187848</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="46">
+        <v>32</v>
+      </c>
+      <c r="B39" s="47" t="s">
+        <v>977</v>
+      </c>
+      <c r="C39" s="47" t="s">
+        <v>784</v>
+      </c>
+      <c r="D39" s="48">
+        <v>44993</v>
+      </c>
+      <c r="E39" s="49">
+        <v>1187506</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="46">
+        <v>33</v>
+      </c>
+      <c r="B40" s="47" t="s">
+        <v>978</v>
+      </c>
+      <c r="C40" s="47" t="s">
+        <v>784</v>
+      </c>
+      <c r="D40" s="48">
+        <v>45028</v>
+      </c>
+      <c r="E40" s="49">
+        <v>1186733</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="46">
+        <v>34</v>
+      </c>
+      <c r="B41" s="47" t="s">
+        <v>979</v>
+      </c>
+      <c r="C41" s="47" t="s">
+        <v>785</v>
+      </c>
+      <c r="D41" s="48">
+        <v>45014</v>
+      </c>
+      <c r="E41" s="49">
+        <v>1177718</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="46">
+        <v>35</v>
+      </c>
+      <c r="B42" s="47" t="s">
+        <v>980</v>
+      </c>
+      <c r="C42" s="47" t="s">
+        <v>784</v>
+      </c>
+      <c r="D42" s="48">
+        <v>45147</v>
+      </c>
+      <c r="E42" s="49">
+        <v>1175436</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="46">
+        <v>36</v>
+      </c>
+      <c r="B43" s="47" t="s">
+        <v>981</v>
+      </c>
+      <c r="C43" s="47" t="s">
+        <v>784</v>
+      </c>
+      <c r="D43" s="48">
+        <v>45182</v>
+      </c>
+      <c r="E43" s="49">
+        <v>1153116</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="46">
+        <v>37</v>
+      </c>
+      <c r="B44" s="47" t="s">
+        <v>982</v>
+      </c>
+      <c r="C44" s="47" t="s">
+        <v>784</v>
+      </c>
+      <c r="D44" s="48">
+        <v>45084</v>
+      </c>
+      <c r="E44" s="49">
+        <v>1137001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="46">
+        <v>38</v>
+      </c>
+      <c r="B45" s="47" t="s">
+        <v>983</v>
+      </c>
+      <c r="C45" s="47" t="s">
+        <v>574</v>
+      </c>
+      <c r="D45" s="48">
+        <v>45280</v>
+      </c>
+      <c r="E45" s="49">
+        <v>1114895</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="46">
+        <v>39</v>
+      </c>
+      <c r="B46" s="47" t="s">
+        <v>984</v>
+      </c>
+      <c r="C46" s="47" t="s">
+        <v>785</v>
+      </c>
+      <c r="D46" s="48">
+        <v>44993</v>
+      </c>
+      <c r="E46" s="49">
+        <v>1104070</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="46">
+        <v>40</v>
+      </c>
+      <c r="B47" s="47" t="s">
+        <v>985</v>
+      </c>
+      <c r="C47" s="47" t="s">
+        <v>785</v>
+      </c>
+      <c r="D47" s="48">
+        <v>45203</v>
+      </c>
+      <c r="E47" s="49">
+        <v>1061162</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="46">
+        <v>41</v>
+      </c>
+      <c r="B48" s="47" t="s">
+        <v>986</v>
+      </c>
+      <c r="C48" s="47" t="s">
+        <v>785</v>
+      </c>
+      <c r="D48" s="48">
+        <v>45007</v>
+      </c>
+      <c r="E48" s="49">
+        <v>1057394</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="46">
+        <v>42</v>
+      </c>
+      <c r="B49" s="47" t="s">
+        <v>987</v>
+      </c>
+      <c r="C49" s="47" t="s">
+        <v>784</v>
+      </c>
+      <c r="D49" s="48">
+        <v>45007</v>
+      </c>
+      <c r="E49" s="49">
+        <v>1053885</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="46">
+        <v>43</v>
+      </c>
+      <c r="B50" s="47" t="s">
+        <v>932</v>
+      </c>
+      <c r="C50" s="47" t="s">
+        <v>784</v>
+      </c>
+      <c r="D50" s="48">
+        <v>44902</v>
+      </c>
+      <c r="E50" s="49">
+        <v>1018379</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" location="Sommaire!A1" display="Retour au menu &quot;Films en salles&quot;" xr:uid="{9079131A-90C8-49CB-99B6-36B820A87F7A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:E54"/>
   <sheetViews>
@@ -13108,516 +14849,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29FDBCDE-30D2-430A-B9BF-A90A04697DD5}">
-  <dimension ref="A2:E34"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="5.28515625" customWidth="1"/>
-    <col min="2" max="2" width="50.28515625" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="37" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="45">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="24" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
-        <v>633</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="46">
-        <v>1</v>
-      </c>
-      <c r="B8" s="47" t="s">
-        <v>923</v>
-      </c>
-      <c r="C8" s="47" t="s">
-        <v>784</v>
-      </c>
-      <c r="D8" s="48">
-        <v>44909</v>
-      </c>
-      <c r="E8" s="49">
-        <v>7903232</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="46">
-        <v>2</v>
-      </c>
-      <c r="B9" s="47" t="s">
-        <v>924</v>
-      </c>
-      <c r="C9" s="47" t="s">
-        <v>784</v>
-      </c>
-      <c r="D9" s="48">
-        <v>44706</v>
-      </c>
-      <c r="E9" s="49">
-        <v>6692372</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="46">
-        <v>3</v>
-      </c>
-      <c r="B10" s="47" t="s">
-        <v>925</v>
-      </c>
-      <c r="C10" s="47" t="s">
-        <v>784</v>
-      </c>
-      <c r="D10" s="48">
-        <v>44748</v>
-      </c>
-      <c r="E10" s="49">
-        <v>3915456</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="46">
-        <v>4</v>
-      </c>
-      <c r="B11" s="47" t="s">
-        <v>926</v>
-      </c>
-      <c r="C11" s="47" t="s">
-        <v>574</v>
-      </c>
-      <c r="D11" s="48">
-        <v>44720</v>
-      </c>
-      <c r="E11" s="49">
-        <v>3488451</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="46">
-        <v>5</v>
-      </c>
-      <c r="B12" s="47" t="s">
-        <v>927</v>
-      </c>
-      <c r="C12" s="47" t="s">
-        <v>784</v>
-      </c>
-      <c r="D12" s="48">
-        <v>44874</v>
-      </c>
-      <c r="E12" s="49">
-        <v>3473467</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="46">
-        <v>6</v>
-      </c>
-      <c r="B13" s="47" t="s">
-        <v>928</v>
-      </c>
-      <c r="C13" s="47" t="s">
-        <v>784</v>
-      </c>
-      <c r="D13" s="48">
-        <v>44685</v>
-      </c>
-      <c r="E13" s="49">
-        <v>3290720</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="46">
-        <v>7</v>
-      </c>
-      <c r="B14" s="47" t="s">
-        <v>929</v>
-      </c>
-      <c r="C14" s="47" t="s">
-        <v>574</v>
-      </c>
-      <c r="D14" s="48">
-        <v>44622</v>
-      </c>
-      <c r="E14" s="49">
-        <v>3040406</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="46">
-        <v>8</v>
-      </c>
-      <c r="B15" s="47" t="s">
-        <v>930</v>
-      </c>
-      <c r="C15" s="47" t="s">
-        <v>784</v>
-      </c>
-      <c r="D15" s="48">
-        <v>44755</v>
-      </c>
-      <c r="E15" s="49">
-        <v>2855490</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="46">
-        <v>9</v>
-      </c>
-      <c r="B16" s="47" t="s">
-        <v>931</v>
-      </c>
-      <c r="C16" s="47" t="s">
-        <v>574</v>
-      </c>
-      <c r="D16" s="48">
-        <v>44664</v>
-      </c>
-      <c r="E16" s="49">
-        <v>2773095</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="46">
-        <v>10</v>
-      </c>
-      <c r="B17" s="47" t="s">
-        <v>932</v>
-      </c>
-      <c r="C17" s="47" t="s">
-        <v>784</v>
-      </c>
-      <c r="D17" s="48">
-        <v>44608</v>
-      </c>
-      <c r="E17" s="49">
-        <v>2507878</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="46">
-        <v>11</v>
-      </c>
-      <c r="B18" s="47" t="s">
-        <v>933</v>
-      </c>
-      <c r="C18" s="47" t="s">
-        <v>785</v>
-      </c>
-      <c r="D18" s="48">
-        <v>44657</v>
-      </c>
-      <c r="E18" s="49">
-        <v>2445139</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="46">
-        <v>12</v>
-      </c>
-      <c r="B19" s="47" t="s">
-        <v>934</v>
-      </c>
-      <c r="C19" s="47" t="s">
-        <v>785</v>
-      </c>
-      <c r="D19" s="48">
-        <v>44839</v>
-      </c>
-      <c r="E19" s="49">
-        <v>2376344</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="46">
-        <v>13</v>
-      </c>
-      <c r="B20" s="47" t="s">
-        <v>935</v>
-      </c>
-      <c r="C20" s="47" t="s">
-        <v>785</v>
-      </c>
-      <c r="D20" s="48">
-        <v>44846</v>
-      </c>
-      <c r="E20" s="49">
-        <v>2304166</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="46">
-        <v>14</v>
-      </c>
-      <c r="B21" s="47" t="s">
-        <v>936</v>
-      </c>
-      <c r="C21" s="47" t="s">
-        <v>784</v>
-      </c>
-      <c r="D21" s="48">
-        <v>44650</v>
-      </c>
-      <c r="E21" s="49">
-        <v>2247767</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="46">
-        <v>15</v>
-      </c>
-      <c r="B22" s="47" t="s">
-        <v>937</v>
-      </c>
-      <c r="C22" s="47" t="s">
-        <v>784</v>
-      </c>
-      <c r="D22" s="48">
-        <v>44853</v>
-      </c>
-      <c r="E22" s="49">
-        <v>2081503</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="46">
-        <v>16</v>
-      </c>
-      <c r="B23" s="47" t="s">
-        <v>938</v>
-      </c>
-      <c r="C23" s="47" t="s">
-        <v>785</v>
-      </c>
-      <c r="D23" s="48">
-        <v>44608</v>
-      </c>
-      <c r="E23" s="49">
-        <v>2036441</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="46">
-        <v>17</v>
-      </c>
-      <c r="B24" s="47" t="s">
-        <v>939</v>
-      </c>
-      <c r="C24" s="47" t="s">
-        <v>784</v>
-      </c>
-      <c r="D24" s="48">
-        <v>44902</v>
-      </c>
-      <c r="E24" s="49">
-        <v>1916378</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="46">
-        <v>18</v>
-      </c>
-      <c r="B25" s="47" t="s">
-        <v>940</v>
-      </c>
-      <c r="C25" s="47" t="s">
-        <v>785</v>
-      </c>
-      <c r="D25" s="48">
-        <v>44594</v>
-      </c>
-      <c r="E25" s="49">
-        <v>1801153</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="46">
-        <v>19</v>
-      </c>
-      <c r="B26" s="47" t="s">
-        <v>941</v>
-      </c>
-      <c r="C26" s="47" t="s">
-        <v>784</v>
-      </c>
-      <c r="D26" s="48">
-        <v>44776</v>
-      </c>
-      <c r="E26" s="49">
-        <v>1533930</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="46">
-        <v>20</v>
-      </c>
-      <c r="B27" s="47" t="s">
-        <v>942</v>
-      </c>
-      <c r="C27" s="47" t="s">
-        <v>784</v>
-      </c>
-      <c r="D27" s="48">
-        <v>44734</v>
-      </c>
-      <c r="E27" s="49">
-        <v>1504203</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="46">
-        <v>21</v>
-      </c>
-      <c r="B28" s="47" t="s">
-        <v>943</v>
-      </c>
-      <c r="C28" s="47" t="s">
-        <v>785</v>
-      </c>
-      <c r="D28" s="48">
-        <v>44650</v>
-      </c>
-      <c r="E28" s="49">
-        <v>1391986</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="46">
-        <v>22</v>
-      </c>
-      <c r="B29" s="47" t="s">
-        <v>944</v>
-      </c>
-      <c r="C29" s="47" t="s">
-        <v>575</v>
-      </c>
-      <c r="D29" s="48">
-        <v>44594</v>
-      </c>
-      <c r="E29" s="49">
-        <v>1339901</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="46">
-        <v>23</v>
-      </c>
-      <c r="B30" s="47" t="s">
-        <v>945</v>
-      </c>
-      <c r="C30" s="47" t="s">
-        <v>784</v>
-      </c>
-      <c r="D30" s="48">
-        <v>44832</v>
-      </c>
-      <c r="E30" s="49">
-        <v>1225450</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="46">
-        <v>24</v>
-      </c>
-      <c r="B31" s="47" t="s">
-        <v>946</v>
-      </c>
-      <c r="C31" s="47" t="s">
-        <v>922</v>
-      </c>
-      <c r="D31" s="48">
-        <v>44734</v>
-      </c>
-      <c r="E31" s="49">
-        <v>1218411</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="46">
-        <v>25</v>
-      </c>
-      <c r="B32" s="47" t="s">
-        <v>947</v>
-      </c>
-      <c r="C32" s="47" t="s">
-        <v>784</v>
-      </c>
-      <c r="D32" s="48">
-        <v>44769</v>
-      </c>
-      <c r="E32" s="49">
-        <v>1166522</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="46">
-        <v>26</v>
-      </c>
-      <c r="B33" s="47" t="s">
-        <v>948</v>
-      </c>
-      <c r="C33" s="47" t="s">
-        <v>785</v>
-      </c>
-      <c r="D33" s="48">
-        <v>44755</v>
-      </c>
-      <c r="E33" s="49">
-        <v>1133183</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="46">
-        <v>27</v>
-      </c>
-      <c r="B34" s="47" t="s">
-        <v>949</v>
-      </c>
-      <c r="C34" s="47" t="s">
-        <v>784</v>
-      </c>
-      <c r="D34" s="48">
-        <v>44657</v>
-      </c>
-      <c r="E34" s="49">
-        <v>1113546</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" location="Sommaire!A1" display="Retour au menu &quot;Films en salles&quot;" xr:uid="{907464C9-CF63-499C-B437-57CFB05611EB}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:E59"/>
   <sheetViews>
@@ -14569,7 +15801,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:E55"/>
   <sheetViews>
@@ -15453,7 +16685,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FF24690-E2BC-49B9-B011-5B4F2DF393CF}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -15467,12 +16699,553 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29FDBCDE-30D2-430A-B9BF-A90A04697DD5}">
+  <dimension ref="A2:E36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.28515625" customWidth="1"/>
+    <col min="2" max="2" width="50.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="37" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="45">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>633</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="46">
+        <v>1</v>
+      </c>
+      <c r="B8" s="47" t="s">
+        <v>916</v>
+      </c>
+      <c r="C8" s="47" t="s">
+        <v>784</v>
+      </c>
+      <c r="D8" s="48">
+        <v>44909</v>
+      </c>
+      <c r="E8" s="49">
+        <v>7906710</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="46">
+        <v>2</v>
+      </c>
+      <c r="B9" s="47" t="s">
+        <v>917</v>
+      </c>
+      <c r="C9" s="47" t="s">
+        <v>784</v>
+      </c>
+      <c r="D9" s="48">
+        <v>44706</v>
+      </c>
+      <c r="E9" s="49">
+        <v>6692490</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="46">
+        <v>3</v>
+      </c>
+      <c r="B10" s="47" t="s">
+        <v>918</v>
+      </c>
+      <c r="C10" s="47" t="s">
+        <v>784</v>
+      </c>
+      <c r="D10" s="48">
+        <v>44748</v>
+      </c>
+      <c r="E10" s="49">
+        <v>3915698</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="46">
+        <v>4</v>
+      </c>
+      <c r="B11" s="47" t="s">
+        <v>919</v>
+      </c>
+      <c r="C11" s="47" t="s">
+        <v>574</v>
+      </c>
+      <c r="D11" s="48">
+        <v>44720</v>
+      </c>
+      <c r="E11" s="49">
+        <v>3488705</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="46">
+        <v>5</v>
+      </c>
+      <c r="B12" s="47" t="s">
+        <v>920</v>
+      </c>
+      <c r="C12" s="47" t="s">
+        <v>784</v>
+      </c>
+      <c r="D12" s="48">
+        <v>44874</v>
+      </c>
+      <c r="E12" s="49">
+        <v>3475710</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="46">
+        <v>6</v>
+      </c>
+      <c r="B13" s="47" t="s">
+        <v>921</v>
+      </c>
+      <c r="C13" s="47" t="s">
+        <v>784</v>
+      </c>
+      <c r="D13" s="48">
+        <v>44685</v>
+      </c>
+      <c r="E13" s="49">
+        <v>3291042</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="46">
+        <v>7</v>
+      </c>
+      <c r="B14" s="47" t="s">
+        <v>922</v>
+      </c>
+      <c r="C14" s="47" t="s">
+        <v>574</v>
+      </c>
+      <c r="D14" s="48">
+        <v>44622</v>
+      </c>
+      <c r="E14" s="49">
+        <v>3040471</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="46">
+        <v>8</v>
+      </c>
+      <c r="B15" s="47" t="s">
+        <v>923</v>
+      </c>
+      <c r="C15" s="47" t="s">
+        <v>784</v>
+      </c>
+      <c r="D15" s="48">
+        <v>44755</v>
+      </c>
+      <c r="E15" s="49">
+        <v>2856065</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="46">
+        <v>9</v>
+      </c>
+      <c r="B16" s="47" t="s">
+        <v>924</v>
+      </c>
+      <c r="C16" s="47" t="s">
+        <v>574</v>
+      </c>
+      <c r="D16" s="48">
+        <v>44664</v>
+      </c>
+      <c r="E16" s="49">
+        <v>2773153</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="46">
+        <v>10</v>
+      </c>
+      <c r="B17" s="47" t="s">
+        <v>925</v>
+      </c>
+      <c r="C17" s="47" t="s">
+        <v>784</v>
+      </c>
+      <c r="D17" s="48">
+        <v>44608</v>
+      </c>
+      <c r="E17" s="49">
+        <v>2507928</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="46">
+        <v>11</v>
+      </c>
+      <c r="B18" s="47" t="s">
+        <v>926</v>
+      </c>
+      <c r="C18" s="47" t="s">
+        <v>785</v>
+      </c>
+      <c r="D18" s="48">
+        <v>44657</v>
+      </c>
+      <c r="E18" s="49">
+        <v>2445189</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="46">
+        <v>12</v>
+      </c>
+      <c r="B19" s="47" t="s">
+        <v>927</v>
+      </c>
+      <c r="C19" s="47" t="s">
+        <v>785</v>
+      </c>
+      <c r="D19" s="48">
+        <v>44839</v>
+      </c>
+      <c r="E19" s="49">
+        <v>2376565</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="46">
+        <v>13</v>
+      </c>
+      <c r="B20" s="47" t="s">
+        <v>928</v>
+      </c>
+      <c r="C20" s="47" t="s">
+        <v>785</v>
+      </c>
+      <c r="D20" s="48">
+        <v>44846</v>
+      </c>
+      <c r="E20" s="49">
+        <v>2304897</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="46">
+        <v>14</v>
+      </c>
+      <c r="B21" s="47" t="s">
+        <v>929</v>
+      </c>
+      <c r="C21" s="47" t="s">
+        <v>784</v>
+      </c>
+      <c r="D21" s="48">
+        <v>44650</v>
+      </c>
+      <c r="E21" s="49">
+        <v>2248022</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="46">
+        <v>15</v>
+      </c>
+      <c r="B22" s="47" t="s">
+        <v>895</v>
+      </c>
+      <c r="C22" s="47" t="s">
+        <v>784</v>
+      </c>
+      <c r="D22" s="48">
+        <v>44545</v>
+      </c>
+      <c r="E22" s="49">
+        <v>2092098</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="46">
+        <v>16</v>
+      </c>
+      <c r="B23" s="47" t="s">
+        <v>930</v>
+      </c>
+      <c r="C23" s="47" t="s">
+        <v>785</v>
+      </c>
+      <c r="D23" s="48">
+        <v>44853</v>
+      </c>
+      <c r="E23" s="49">
+        <v>2081640</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="46">
+        <v>17</v>
+      </c>
+      <c r="B24" s="47" t="s">
+        <v>931</v>
+      </c>
+      <c r="C24" s="47" t="s">
+        <v>784</v>
+      </c>
+      <c r="D24" s="48">
+        <v>44608</v>
+      </c>
+      <c r="E24" s="49">
+        <v>2036613</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="46">
+        <v>18</v>
+      </c>
+      <c r="B25" s="47" t="s">
+        <v>932</v>
+      </c>
+      <c r="C25" s="47" t="s">
+        <v>785</v>
+      </c>
+      <c r="D25" s="48">
+        <v>44902</v>
+      </c>
+      <c r="E25" s="49">
+        <v>1917621</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="46">
+        <v>19</v>
+      </c>
+      <c r="B26" s="47" t="s">
+        <v>933</v>
+      </c>
+      <c r="C26" s="47" t="s">
+        <v>784</v>
+      </c>
+      <c r="D26" s="48">
+        <v>44594</v>
+      </c>
+      <c r="E26" s="49">
+        <v>1801232</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="46">
+        <v>20</v>
+      </c>
+      <c r="B27" s="47" t="s">
+        <v>934</v>
+      </c>
+      <c r="C27" s="47" t="s">
+        <v>784</v>
+      </c>
+      <c r="D27" s="48">
+        <v>44776</v>
+      </c>
+      <c r="E27" s="49">
+        <v>1534142</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="46">
+        <v>21</v>
+      </c>
+      <c r="B28" s="47" t="s">
+        <v>935</v>
+      </c>
+      <c r="C28" s="47" t="s">
+        <v>785</v>
+      </c>
+      <c r="D28" s="48">
+        <v>44734</v>
+      </c>
+      <c r="E28" s="49">
+        <v>1504265</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="46">
+        <v>22</v>
+      </c>
+      <c r="B29" s="47" t="s">
+        <v>936</v>
+      </c>
+      <c r="C29" s="47" t="s">
+        <v>575</v>
+      </c>
+      <c r="D29" s="48">
+        <v>44650</v>
+      </c>
+      <c r="E29" s="49">
+        <v>1392035</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="46">
+        <v>23</v>
+      </c>
+      <c r="B30" s="47" t="s">
+        <v>937</v>
+      </c>
+      <c r="C30" s="47" t="s">
+        <v>784</v>
+      </c>
+      <c r="D30" s="48">
+        <v>44594</v>
+      </c>
+      <c r="E30" s="49">
+        <v>1339901</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="46">
+        <v>24</v>
+      </c>
+      <c r="B31" s="47" t="s">
+        <v>938</v>
+      </c>
+      <c r="C31" s="47" t="s">
+        <v>915</v>
+      </c>
+      <c r="D31" s="48">
+        <v>44832</v>
+      </c>
+      <c r="E31" s="49">
+        <v>1225339</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="46">
+        <v>25</v>
+      </c>
+      <c r="B32" s="47" t="s">
+        <v>939</v>
+      </c>
+      <c r="C32" s="47" t="s">
+        <v>784</v>
+      </c>
+      <c r="D32" s="48">
+        <v>44734</v>
+      </c>
+      <c r="E32" s="49">
+        <v>1218677</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="46">
+        <v>26</v>
+      </c>
+      <c r="B33" s="47" t="s">
+        <v>940</v>
+      </c>
+      <c r="C33" s="47" t="s">
+        <v>785</v>
+      </c>
+      <c r="D33" s="48">
+        <v>44769</v>
+      </c>
+      <c r="E33" s="49">
+        <v>1166865</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="46">
+        <v>27</v>
+      </c>
+      <c r="B34" s="47" t="s">
+        <v>941</v>
+      </c>
+      <c r="C34" s="47" t="s">
+        <v>784</v>
+      </c>
+      <c r="D34" s="48">
+        <v>44755</v>
+      </c>
+      <c r="E34" s="49">
+        <v>1133649</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="46">
+        <v>28</v>
+      </c>
+      <c r="B35" s="47" t="s">
+        <v>942</v>
+      </c>
+      <c r="C35" s="47" t="s">
+        <v>785</v>
+      </c>
+      <c r="D35" s="48">
+        <v>44657</v>
+      </c>
+      <c r="E35" s="49">
+        <v>1113796</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="46">
+        <v>29</v>
+      </c>
+      <c r="B36" s="47" t="s">
+        <v>912</v>
+      </c>
+      <c r="C36" s="47" t="s">
+        <v>784</v>
+      </c>
+      <c r="D36" s="48">
+        <v>44552</v>
+      </c>
+      <c r="E36" s="49">
+        <v>1092488</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" location="Sommaire!A1" display="Retour au menu &quot;Films en salles&quot;" xr:uid="{907464C9-CF63-499C-B437-57CFB05611EB}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CF6726B-45BA-4F5A-921F-7CB9D98E094C}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
@@ -15560,7 +17333,7 @@
         <v>44545</v>
       </c>
       <c r="E8" s="19">
-        <v>4581507</v>
+        <v>4590410</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -15577,7 +17350,7 @@
         <v>44475</v>
       </c>
       <c r="E9" s="19">
-        <v>3996589</v>
+        <v>3997921</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -15594,7 +17367,7 @@
         <v>44454</v>
       </c>
       <c r="E10" s="19">
-        <v>3178018</v>
+        <v>3178755</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -15602,7 +17375,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>898</v>
+        <v>988</v>
       </c>
       <c r="C11" s="17" t="s">
         <v>785</v>
@@ -15611,7 +17384,7 @@
         <v>44398</v>
       </c>
       <c r="E11" s="19">
-        <v>2656445</v>
+        <v>2657944</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -15619,7 +17392,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>785</v>
@@ -15628,7 +17401,7 @@
         <v>44426</v>
       </c>
       <c r="E12" s="19">
-        <v>2210902</v>
+        <v>2211573</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -15636,7 +17409,7 @@
         <v>6</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>784</v>
@@ -15645,7 +17418,7 @@
         <v>44524</v>
       </c>
       <c r="E13" s="19">
-        <v>2206683</v>
+        <v>2209990</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -15653,7 +17426,7 @@
         <v>7</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>901</v>
+        <v>989</v>
       </c>
       <c r="C14" s="17" t="s">
         <v>574</v>
@@ -15662,7 +17435,7 @@
         <v>44391</v>
       </c>
       <c r="E14" s="19">
-        <v>1987918</v>
+        <v>1988342</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -15670,7 +17443,7 @@
         <v>8</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>902</v>
+        <v>990</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>785</v>
@@ -15679,7 +17452,7 @@
         <v>44538</v>
       </c>
       <c r="E15" s="19">
-        <v>1940774</v>
+        <v>1945688</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -15687,7 +17460,7 @@
         <v>9</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>903</v>
+        <v>991</v>
       </c>
       <c r="C16" s="17" t="s">
         <v>784</v>
@@ -15696,7 +17469,7 @@
         <v>44356</v>
       </c>
       <c r="E16" s="19">
-        <v>1885246</v>
+        <v>1885466</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -15704,7 +17477,7 @@
         <v>10</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>904</v>
+        <v>900</v>
       </c>
       <c r="C17" s="17" t="s">
         <v>784</v>
@@ -15713,7 +17486,7 @@
         <v>44503</v>
       </c>
       <c r="E17" s="19">
-        <v>1712234</v>
+        <v>1713052</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -15721,7 +17494,7 @@
         <v>11</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>905</v>
+        <v>901</v>
       </c>
       <c r="C18" s="17" t="s">
         <v>784</v>
@@ -15730,7 +17503,7 @@
         <v>44384</v>
       </c>
       <c r="E18" s="19">
-        <v>1677619</v>
+        <v>1678054</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -15738,7 +17511,7 @@
         <v>12</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>906</v>
+        <v>902</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>784</v>
@@ -15747,7 +17520,7 @@
         <v>44489</v>
       </c>
       <c r="E19" s="19">
-        <v>1623878</v>
+        <v>1624631</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -15755,7 +17528,7 @@
         <v>13</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>907</v>
+        <v>903</v>
       </c>
       <c r="C20" s="17" t="s">
         <v>785</v>
@@ -15764,7 +17537,7 @@
         <v>44412</v>
       </c>
       <c r="E20" s="19">
-        <v>1623601</v>
+        <v>1624567</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -15772,7 +17545,7 @@
         <v>14</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>908</v>
+        <v>992</v>
       </c>
       <c r="C21" s="17" t="s">
         <v>785</v>
@@ -15781,7 +17554,7 @@
         <v>44517</v>
       </c>
       <c r="E21" s="19">
-        <v>1500886</v>
+        <v>1505722</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -15789,16 +17562,16 @@
         <v>15</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>909</v>
+        <v>904</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>910</v>
+        <v>905</v>
       </c>
       <c r="D22" s="18">
         <v>44482</v>
       </c>
       <c r="E22" s="19">
-        <v>1493558</v>
+        <v>1494551</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -15806,7 +17579,7 @@
         <v>16</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>911</v>
+        <v>993</v>
       </c>
       <c r="C23" s="17" t="s">
         <v>784</v>
@@ -15815,7 +17588,7 @@
         <v>44419</v>
       </c>
       <c r="E23" s="19">
-        <v>1473730</v>
+        <v>1473865</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -15823,7 +17596,7 @@
         <v>17</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>912</v>
+        <v>906</v>
       </c>
       <c r="C24" s="17" t="s">
         <v>784</v>
@@ -15832,7 +17605,7 @@
         <v>44370</v>
       </c>
       <c r="E24" s="19">
-        <v>1426229</v>
+        <v>1426572</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -15840,7 +17613,7 @@
         <v>18</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>913</v>
+        <v>907</v>
       </c>
       <c r="C25" s="17" t="s">
         <v>784</v>
@@ -15849,7 +17622,7 @@
         <v>44440</v>
       </c>
       <c r="E25" s="19">
-        <v>1379799</v>
+        <v>1379926</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -15857,7 +17630,7 @@
         <v>19</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>914</v>
+        <v>908</v>
       </c>
       <c r="C26" s="17" t="s">
         <v>785</v>
@@ -15866,7 +17639,7 @@
         <v>44125</v>
       </c>
       <c r="E26" s="19">
-        <v>1286046</v>
+        <v>1286461</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -15874,16 +17647,16 @@
         <v>20</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>915</v>
+        <v>909</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>916</v>
+        <v>910</v>
       </c>
       <c r="D27" s="18">
         <v>44510</v>
       </c>
       <c r="E27" s="19">
-        <v>1276629</v>
+        <v>1277445</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -15891,7 +17664,7 @@
         <v>21</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>917</v>
+        <v>911</v>
       </c>
       <c r="C28" s="17" t="s">
         <v>785</v>
@@ -15900,7 +17673,7 @@
         <v>44447</v>
       </c>
       <c r="E28" s="19">
-        <v>1182706</v>
+        <v>1183583</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -15908,16 +17681,16 @@
         <v>22</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>918</v>
+        <v>994</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>916</v>
+        <v>910</v>
       </c>
       <c r="D29" s="18">
         <v>44482</v>
       </c>
       <c r="E29" s="19">
-        <v>1173707</v>
+        <v>1174773</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -15925,7 +17698,7 @@
         <v>23</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>919</v>
+        <v>912</v>
       </c>
       <c r="C30" s="17" t="s">
         <v>784</v>
@@ -15934,7 +17707,7 @@
         <v>44552</v>
       </c>
       <c r="E30" s="19">
-        <v>1169311</v>
+        <v>1170338</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -15942,7 +17715,7 @@
         <v>24</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>920</v>
+        <v>913</v>
       </c>
       <c r="C31" s="17" t="s">
         <v>784</v>
@@ -15951,7 +17724,7 @@
         <v>44384</v>
       </c>
       <c r="E31" s="19">
-        <v>1132485</v>
+        <v>1132826</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -15959,7 +17732,7 @@
         <v>25</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>921</v>
+        <v>914</v>
       </c>
       <c r="C32" s="17" t="s">
         <v>784</v>
@@ -15968,7 +17741,7 @@
         <v>44426</v>
       </c>
       <c r="E32" s="19">
-        <v>1008633</v>
+        <v>1009451</v>
       </c>
     </row>
   </sheetData>
@@ -15979,7 +17752,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9D84FE3-27EA-42FC-A266-0E9729DD5E9F}">
   <dimension ref="A1:E20"/>
   <sheetViews>
@@ -16286,7 +18059,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7289E66B-29F5-47E9-A60C-E2ADE2B77D4A}">
   <dimension ref="A1:E58"/>
   <sheetViews>
@@ -17239,7 +19012,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B1BEF9C-F365-49B1-AC20-4E7810EC2710}">
   <dimension ref="A1:E49"/>
   <sheetViews>
@@ -18039,7 +19812,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E63"/>
   <sheetViews>
@@ -18601,7 +20374,7 @@
         <v>758</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>922</v>
+        <v>915</v>
       </c>
       <c r="D36" s="18">
         <v>42788</v>
@@ -19077,7 +20850,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E61"/>
   <sheetViews>
@@ -20068,844 +21841,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E52"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="5.28515625" style="24" customWidth="1"/>
-    <col min="2" max="2" width="50.28515625" style="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.140625" style="34" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" style="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" style="27" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:5" s="37" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-    </row>
-    <row r="3" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="6">
-        <v>2015</v>
-      </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="9"/>
-    </row>
-    <row r="6" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="9"/>
-    </row>
-    <row r="7" spans="1:5" ht="24" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
-        <v>633</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="16">
-        <v>1</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>634</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="18">
-        <v>42354</v>
-      </c>
-      <c r="E8" s="19">
-        <v>7327435</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="16">
-        <v>2</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>716</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="18">
-        <v>42193</v>
-      </c>
-      <c r="E9" s="19">
-        <v>6655855</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="16">
-        <v>3</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>717</v>
-      </c>
-      <c r="C10" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="18">
-        <v>41990</v>
-      </c>
-      <c r="E10" s="19">
-        <v>5351811</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="16">
-        <v>4</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>635</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="18">
-        <v>42165</v>
-      </c>
-      <c r="E11" s="19">
-        <v>5214046</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="16">
-        <v>5</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>636</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="18">
-        <v>42319</v>
-      </c>
-      <c r="E12" s="19">
-        <v>4813082</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="16">
-        <v>6</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>637</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="18">
-        <v>42095</v>
-      </c>
-      <c r="E13" s="19">
-        <v>4631125</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="16">
-        <v>7</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>718</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="18">
-        <v>42291</v>
-      </c>
-      <c r="E14" s="19">
-        <v>4426102</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="16">
-        <v>8</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>638</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="18">
-        <v>42172</v>
-      </c>
-      <c r="E15" s="19">
-        <v>4410201</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="16">
-        <v>9</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>639</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="18">
-        <v>42116</v>
-      </c>
-      <c r="E16" s="19">
-        <v>4240121</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="16">
-        <v>10</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>640</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="18">
-        <v>42046</v>
-      </c>
-      <c r="E17" s="19">
-        <v>4065415</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="16">
-        <v>11</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>719</v>
-      </c>
-      <c r="C18" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="18">
-        <v>42186</v>
-      </c>
-      <c r="E18" s="19">
-        <v>3494441</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="16">
-        <v>12</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>641</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="18">
-        <v>42053</v>
-      </c>
-      <c r="E19" s="19">
-        <v>3132953</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="16">
-        <v>13</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>720</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="18">
-        <v>42284</v>
-      </c>
-      <c r="E20" s="19">
-        <v>3122000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="16">
-        <v>14</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>642</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="18">
-        <v>42039</v>
-      </c>
-      <c r="E21" s="19">
-        <v>2887691</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="16">
-        <v>15</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>643</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="18">
-        <v>42228</v>
-      </c>
-      <c r="E22" s="19">
-        <v>2797975</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="16">
-        <v>16</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>721</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" s="18">
-        <v>42326</v>
-      </c>
-      <c r="E23" s="19">
-        <v>2773963</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="16">
-        <v>17</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>644</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="18">
-        <v>42025</v>
-      </c>
-      <c r="E24" s="19">
-        <v>2612213</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="16">
-        <v>18</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>645</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" s="18">
-        <v>42340</v>
-      </c>
-      <c r="E25" s="19">
-        <v>2525612</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="16">
-        <v>19</v>
-      </c>
-      <c r="B26" s="17" t="s">
-        <v>646</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26" s="18">
-        <v>42298</v>
-      </c>
-      <c r="E26" s="19">
-        <v>2519790</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="16">
-        <v>20</v>
-      </c>
-      <c r="B27" s="17" t="s">
-        <v>647</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D27" s="18">
-        <v>42081</v>
-      </c>
-      <c r="E27" s="19">
-        <v>2417013</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="16">
-        <v>21</v>
-      </c>
-      <c r="B28" s="17" t="s">
-        <v>648</v>
-      </c>
-      <c r="C28" s="29" t="s">
-        <v>170</v>
-      </c>
-      <c r="D28" s="18">
-        <v>42102</v>
-      </c>
-      <c r="E28" s="19">
-        <v>2410643</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="16">
-        <v>22</v>
-      </c>
-      <c r="B29" s="17" t="s">
-        <v>649</v>
-      </c>
-      <c r="C29" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="D29" s="18">
-        <v>42138</v>
-      </c>
-      <c r="E29" s="19">
-        <v>2359477</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="16">
-        <v>23</v>
-      </c>
-      <c r="B30" s="17" t="s">
-        <v>722</v>
-      </c>
-      <c r="C30" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D30" s="18">
-        <v>42333</v>
-      </c>
-      <c r="E30" s="19">
-        <v>2316475</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="16">
-        <v>24</v>
-      </c>
-      <c r="B31" s="17" t="s">
-        <v>650</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D31" s="18">
-        <v>42284</v>
-      </c>
-      <c r="E31" s="19">
-        <v>2298078</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="16">
-        <v>25</v>
-      </c>
-      <c r="B32" s="17" t="s">
-        <v>723</v>
-      </c>
-      <c r="C32" s="29" t="s">
-        <v>170</v>
-      </c>
-      <c r="D32" s="18">
-        <v>42214</v>
-      </c>
-      <c r="E32" s="19">
-        <v>1934437</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="16">
-        <v>26</v>
-      </c>
-      <c r="B33" s="17" t="s">
-        <v>651</v>
-      </c>
-      <c r="C33" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D33" s="18">
-        <v>42199</v>
-      </c>
-      <c r="E33" s="19">
-        <v>1721905</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="16">
-        <v>27</v>
-      </c>
-      <c r="B34" s="17" t="s">
-        <v>652</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="D34" s="18">
-        <v>42088</v>
-      </c>
-      <c r="E34" s="19">
-        <v>1674276</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="16">
-        <v>28</v>
-      </c>
-      <c r="B35" s="17" t="s">
-        <v>653</v>
-      </c>
-      <c r="C35" s="29" t="s">
-        <v>729</v>
-      </c>
-      <c r="D35" s="18">
-        <v>42053</v>
-      </c>
-      <c r="E35" s="19">
-        <v>1666999</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="16">
-        <v>29</v>
-      </c>
-      <c r="B36" s="17" t="s">
-        <v>724</v>
-      </c>
-      <c r="C36" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D36" s="18">
-        <v>42046</v>
-      </c>
-      <c r="E36" s="19">
-        <v>1660709</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="16">
-        <v>30</v>
-      </c>
-      <c r="B37" s="17" t="s">
-        <v>725</v>
-      </c>
-      <c r="C37" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D37" s="18">
-        <v>42039</v>
-      </c>
-      <c r="E37" s="19">
-        <v>1591922</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="16">
-        <v>31</v>
-      </c>
-      <c r="B38" s="17" t="s">
-        <v>654</v>
-      </c>
-      <c r="C38" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="D38" s="18">
-        <v>42053</v>
-      </c>
-      <c r="E38" s="19">
-        <v>1512366</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="16">
-        <v>32</v>
-      </c>
-      <c r="B39" s="17" t="s">
-        <v>655</v>
-      </c>
-      <c r="C39" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D39" s="18">
-        <v>42186</v>
-      </c>
-      <c r="E39" s="19">
-        <v>1425869</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="16">
-        <v>33</v>
-      </c>
-      <c r="B40" s="17" t="s">
-        <v>726</v>
-      </c>
-      <c r="C40" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="D40" s="18">
-        <v>42347</v>
-      </c>
-      <c r="E40" s="19">
-        <v>1369011</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="16">
-        <v>34</v>
-      </c>
-      <c r="B41" s="17" t="s">
-        <v>727</v>
-      </c>
-      <c r="C41" s="29" t="s">
-        <v>730</v>
-      </c>
-      <c r="D41" s="18">
-        <v>42060</v>
-      </c>
-      <c r="E41" s="19">
-        <v>1326539</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="16">
-        <v>35</v>
-      </c>
-      <c r="B42" s="17" t="s">
-        <v>656</v>
-      </c>
-      <c r="C42" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D42" s="18">
-        <v>42053</v>
-      </c>
-      <c r="E42" s="19">
-        <v>1300935</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="16">
-        <v>36</v>
-      </c>
-      <c r="B43" s="17" t="s">
-        <v>657</v>
-      </c>
-      <c r="C43" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D43" s="18">
-        <v>42109</v>
-      </c>
-      <c r="E43" s="19">
-        <v>1224306</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="16">
-        <v>37</v>
-      </c>
-      <c r="B44" s="17" t="s">
-        <v>279</v>
-      </c>
-      <c r="C44" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D44" s="18">
-        <v>42221</v>
-      </c>
-      <c r="E44" s="19">
-        <v>1204400</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="16">
-        <v>38</v>
-      </c>
-      <c r="B45" s="17" t="s">
-        <v>658</v>
-      </c>
-      <c r="C45" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="D45" s="18">
-        <v>42123</v>
-      </c>
-      <c r="E45" s="19">
-        <v>1199076</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="16">
-        <v>39</v>
-      </c>
-      <c r="B46" s="17" t="s">
-        <v>659</v>
-      </c>
-      <c r="C46" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D46" s="18">
-        <v>42151</v>
-      </c>
-      <c r="E46" s="19">
-        <v>1151362</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="16">
-        <v>40</v>
-      </c>
-      <c r="B47" s="17" t="s">
-        <v>660</v>
-      </c>
-      <c r="C47" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D47" s="18">
-        <v>42221</v>
-      </c>
-      <c r="E47" s="19">
-        <v>1143896</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="16">
-        <v>41</v>
-      </c>
-      <c r="B48" s="17" t="s">
-        <v>661</v>
-      </c>
-      <c r="C48" s="29" t="s">
-        <v>729</v>
-      </c>
-      <c r="D48" s="18">
-        <v>42032</v>
-      </c>
-      <c r="E48" s="19">
-        <v>1088829</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" s="16">
-        <v>42</v>
-      </c>
-      <c r="B49" s="17" t="s">
-        <v>662</v>
-      </c>
-      <c r="C49" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="D49" s="18">
-        <v>42095</v>
-      </c>
-      <c r="E49" s="19">
-        <v>1063446</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" s="16">
-        <v>43</v>
-      </c>
-      <c r="B50" s="17" t="s">
-        <v>728</v>
-      </c>
-      <c r="C50" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="D50" s="18">
-        <v>42018</v>
-      </c>
-      <c r="E50" s="19">
-        <v>1062983</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" s="16">
-        <v>44</v>
-      </c>
-      <c r="B51" s="17" t="s">
-        <v>663</v>
-      </c>
-      <c r="C51" s="29" t="s">
-        <v>731</v>
-      </c>
-      <c r="D51" s="18">
-        <v>42263</v>
-      </c>
-      <c r="E51" s="19">
-        <v>1008223</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" s="23"/>
-      <c r="C52" s="34" t="s">
-        <v>732</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" location="Sommaire!A1" display="Retour au menu &quot;Films en salles&quot;" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>